<commit_message>
Added my collection of parts to inventory list
</commit_message>
<xml_diff>
--- a/docs/Parts List.xlsx
+++ b/docs/Parts List.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jak\win_shared\projs\base_components\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\git_wa\hw-design\base_components\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06134070-3683-40D5-B273-B16FB611CAB1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CC748C2-324B-419B-8578-AF03AB249F33}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{66A120A8-4437-4281-AA28-687631655034}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="57">
   <si>
     <t>47W01TF LMT87</t>
   </si>
@@ -94,6 +94,114 @@
   </si>
   <si>
     <t>SPDT (Single Pole, Double Throw)</t>
+  </si>
+  <si>
+    <t>Jak</t>
+  </si>
+  <si>
+    <t>Josh</t>
+  </si>
+  <si>
+    <t>White text on blue with backlight</t>
+  </si>
+  <si>
+    <t>1848 Motor Driver</t>
+  </si>
+  <si>
+    <t>GY-521 Module</t>
+  </si>
+  <si>
+    <t>1602A 16x2 LCD Display Module</t>
+  </si>
+  <si>
+    <t>MPU-6050 MEMS</t>
+  </si>
+  <si>
+    <t>SSD1306 OLED Display Module</t>
+  </si>
+  <si>
+    <t>I2C 128x32 resolution</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L7805CV </t>
+  </si>
+  <si>
+    <t>5V voltage regulator</t>
+  </si>
+  <si>
+    <t>20MHz Oscillator</t>
+  </si>
+  <si>
+    <t>NEO-6M-0-001</t>
+  </si>
+  <si>
+    <t>GPS Module</t>
+  </si>
+  <si>
+    <t>OV7670 Camera Module</t>
+  </si>
+  <si>
+    <t>640x48- CMOS Sensor</t>
+  </si>
+  <si>
+    <t>Atmel AVRISP Mk2</t>
+  </si>
+  <si>
+    <t>Atmel USB programmer</t>
+  </si>
+  <si>
+    <t>PICkit 3</t>
+  </si>
+  <si>
+    <t>PIC USB programmer</t>
+  </si>
+  <si>
+    <t>4 AA Battery Holder</t>
+  </si>
+  <si>
+    <t>1 AA Battery Holder</t>
+  </si>
+  <si>
+    <t>2 AA Battery Holder</t>
+  </si>
+  <si>
+    <t>2 Pin Tactile Button</t>
+  </si>
+  <si>
+    <t>6x6mm</t>
+  </si>
+  <si>
+    <t>1 Digit 7-Segment Display</t>
+  </si>
+  <si>
+    <t>Color?</t>
+  </si>
+  <si>
+    <t>Resistors</t>
+  </si>
+  <si>
+    <t>Too many</t>
+  </si>
+  <si>
+    <t>Various values</t>
+  </si>
+  <si>
+    <t>Ceramic Capacitors</t>
+  </si>
+  <si>
+    <t>Nokia 1202 LCD Display</t>
+  </si>
+  <si>
+    <t>96x68 resolution</t>
+  </si>
+  <si>
+    <t>Male pin headers</t>
+  </si>
+  <si>
+    <t>40x1 2.54mm pitch</t>
+  </si>
+  <si>
+    <t>Female headers</t>
   </si>
 </sst>
 </file>
@@ -109,15 +217,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -125,15 +239,35 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -448,10 +582,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DB91B24-1720-49EC-B152-221D76E119C6}">
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:E36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -461,145 +595,443 @@
     <col min="3" max="3" width="34.85546875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="D1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1">
-        <v>1</v>
-      </c>
-      <c r="C2" s="1" t="s">
+      <c r="B2" s="2">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="D2" s="3"/>
+      <c r="E2" s="4"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3" s="2">
         <v>3</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="D3" s="3"/>
+      <c r="E3" s="4"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="B4" s="2">
+        <v>1</v>
+      </c>
+      <c r="C4" s="2"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="4"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+      <c r="B5" s="2">
+        <v>1</v>
+      </c>
+      <c r="C5" s="2"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="4"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B6" s="2">
         <v>6</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+      <c r="C6" s="2"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="4"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B7" s="2">
         <v>9</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+      <c r="C7" s="2"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="4"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="1">
+      <c r="B8" s="2">
         <v>9</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+      <c r="C8" s="2"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="4"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="1">
+      <c r="B9" s="2">
         <v>6</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+      <c r="C9" s="2"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="4"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="1">
-        <v>1</v>
-      </c>
-      <c r="C10" s="1" t="s">
+      <c r="B10" s="2">
+        <v>1</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+      <c r="D10" s="3"/>
+      <c r="E10" s="4"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="1">
+      <c r="B11" s="2">
         <v>15</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+      <c r="C11" s="2"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="4"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+      <c r="B12" s="2">
+        <v>1</v>
+      </c>
+      <c r="C12" s="2"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="4"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B13" s="1">
+      <c r="B13" s="2">
         <v>35</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
+      <c r="C13" s="2"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="4"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="1">
+      <c r="B14" s="2">
         <v>4</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
+      <c r="C14" s="2"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="4"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="1">
+      <c r="B15" s="2">
         <v>8</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
+      <c r="C15" s="2"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="4"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B16" s="1">
+      <c r="B16" s="2">
         <v>6</v>
       </c>
+      <c r="C16" s="2"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="4"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17" s="2">
+        <v>2</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D17" s="4"/>
+      <c r="E17" s="3"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B18" s="2">
+        <v>2</v>
+      </c>
+      <c r="C18" s="2"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="3"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B19" s="2">
+        <v>1</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D19" s="4"/>
+      <c r="E19" s="3"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B20" s="2">
+        <v>2</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D20" s="4"/>
+      <c r="E20" s="3"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B21" s="2">
+        <v>1</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D21" s="4"/>
+      <c r="E21" s="3"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B22" s="2">
+        <v>10</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D22" s="4"/>
+      <c r="E22" s="3"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="2"/>
+      <c r="B23" s="2">
+        <v>10</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D23" s="4"/>
+      <c r="E23" s="3"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B24" s="2">
+        <v>1</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D24" s="4"/>
+      <c r="E24" s="3"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B25" s="2">
+        <v>1</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D25" s="4"/>
+      <c r="E25" s="3"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B26" s="2">
+        <v>1</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D26" s="4"/>
+      <c r="E26" s="3"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B27" s="2">
+        <v>1</v>
+      </c>
+      <c r="C27" s="2"/>
+      <c r="D27" s="4"/>
+      <c r="E27" s="3"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B28" s="2">
+        <v>1</v>
+      </c>
+      <c r="C28" s="2"/>
+      <c r="D28" s="4"/>
+      <c r="E28" s="3"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B29" s="2">
+        <v>8</v>
+      </c>
+      <c r="C29" s="2"/>
+      <c r="D29" s="4"/>
+      <c r="E29" s="3"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B30" s="2">
+        <v>15</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D30" s="4"/>
+      <c r="E30" s="3"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B31" s="2">
+        <v>10</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D31" s="4"/>
+      <c r="E31" s="3"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D32" s="4"/>
+      <c r="E32" s="3"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D33" s="2"/>
+      <c r="E33" s="3"/>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B34" s="2">
+        <v>2</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D34" s="4"/>
+      <c r="E34" s="3"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B35" s="2">
+        <v>10</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D35" s="4"/>
+      <c r="E35" s="3"/>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B36" s="2">
+        <v>2</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D36" s="4"/>
+      <c r="E36" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
More items added to inventory list
</commit_message>
<xml_diff>
--- a/docs/Parts List.xlsx
+++ b/docs/Parts List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\git_wa\hw-design\base_components\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CC748C2-324B-419B-8578-AF03AB249F33}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CC835D7-CA49-4233-8980-C5D4FC4F9B13}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{66A120A8-4437-4281-AA28-687631655034}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="60">
   <si>
     <t>47W01TF LMT87</t>
   </si>
@@ -202,6 +202,15 @@
   </si>
   <si>
     <t>Female headers</t>
+  </si>
+  <si>
+    <t>Futaba 3003 Servo</t>
+  </si>
+  <si>
+    <t>Tower Pro SG90</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 9 grams</t>
   </si>
 </sst>
 </file>
@@ -582,10 +591,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DB91B24-1720-49EC-B152-221D76E119C6}">
-  <dimension ref="A1:E36"/>
+  <dimension ref="A1:E38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F38" sqref="F38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1033,6 +1042,30 @@
       <c r="D36" s="4"/>
       <c r="E36" s="3"/>
     </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B37" s="2">
+        <v>8</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D37" s="4"/>
+      <c r="E37" s="3"/>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B38" s="2">
+        <v>10</v>
+      </c>
+      <c r="C38" s="2"/>
+      <c r="D38" s="4"/>
+      <c r="E38" s="3"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>